<commit_message>
Refactor parity generation logic to exclude unnecessary FIERR ports and improve port declaration handling
</commit_message>
<xml_diff>
--- a/simple_test/[INFO]_SIMPLE_TOP.safety.xlsx
+++ b/simple_test/[INFO]_SIMPLE_TOP.safety.xlsx
@@ -2,31 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="SAFETY.PARITY" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
       <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <sz val="8"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -46,10 +56,19 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -62,7 +81,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -427,11 +446,18 @@
   </sheetPr>
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
+  <cols>
+    <col width="12.375" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="22.25" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="21.375" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="23.75" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="20.125" bestFit="1" customWidth="1" min="14" max="14"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -544,9 +570,6 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr">
         <is>
           <t>SIMPLE_TOP</t>
@@ -574,7 +597,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>DRIVE</t>
+          <t>RECEIVE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -597,7 +620,6 @@
           <t>ERR_WADDR_PARITY</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
         <v>32</v>
       </c>
@@ -625,9 +647,6 @@
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>SIMPLE_TOP</t>
@@ -655,7 +674,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>DRIVE</t>
+          <t>RECEIVE</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -678,7 +697,6 @@
           <t>ERR_WDATA_PARITY</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
         <v>64</v>
       </c>
@@ -706,9 +724,6 @@
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr">
         <is>
           <t>SIMPLE_TOP</t>
@@ -736,7 +751,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>DRIVE</t>
+          <t>RECEIVE</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -759,7 +774,6 @@
           <t>ERR_RADDR_PARITY</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
         <v>32</v>
       </c>
@@ -787,9 +801,6 @@
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>SIMPLE_TOP</t>
@@ -817,7 +828,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>RECEIVE</t>
+          <t>DRIVE</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -840,7 +851,6 @@
           <t>ERR_RDATA_PARITY</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
         <v>64</v>
       </c>

</xml_diff>

<commit_message>
Add MD5 and version
</commit_message>
<xml_diff>
--- a/simple_test/[INFO]_SIMPLE_TOP.safety.xlsx
+++ b/simple_test/[INFO]_SIMPLE_TOP.safety.xlsx
@@ -444,7 +444,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -560,7 +560,12 @@
           <t>COMPARATOR DEPTH</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" t="inlineStr">
+        <is>
+          <t>MD5 &amp; Script Version</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>NOTE</t>
         </is>
@@ -639,6 +644,11 @@
       </c>
       <c r="U2" t="inlineStr">
         <is>
+          <t>MD5: 33d07e47ee89e1db338f01228abafde5 | Script: v3.0.0</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
           <t>Write Address Parity</t>
         </is>
       </c>
@@ -716,6 +726,11 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
+          <t>MD5: 2363d6688c56d6cd78be8f9a481fcf8f | Script: v3.0.0</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
           <t>Write Data Parity</t>
         </is>
       </c>
@@ -793,6 +808,11 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
+          <t>MD5: 21b9a9f0d70e550ae3d66ed506ff9e2d | Script: v3.0.0</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
           <t>Read Address Parity</t>
         </is>
       </c>
@@ -869,6 +889,11 @@
         <v>0</v>
       </c>
       <c r="U5" t="inlineStr">
+        <is>
+          <t>MD5: 305f3681692ea4f39d05961cd6714eeb | Script: v3.0.0</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
         <is>
           <t>Read Data Parity</t>
         </is>

</xml_diff>